<commit_message>
Completed the About me page
</commit_message>
<xml_diff>
--- a/database/skills_db_en.xlsx
+++ b/database/skills_db_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navrozlamba/repo/portfolio-navroz/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6A9A72-44A0-BE40-BE93-25DB6B419060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964E66A0-AA7F-7440-B6BC-E95CFE6E94FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49640" yWindow="620" windowWidth="20640" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
+    <workbookView xWindow="49640" yWindow="500" windowWidth="20640" windowHeight="20160" xr2:uid="{BE9CF97B-0840-1748-96CC-677E31A7EECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>topic</t>
   </si>
@@ -54,21 +54,9 @@
     <t>id</t>
   </si>
   <si>
-    <t>python</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>helper.get_title_content</t>
-  </si>
-  <si>
-    <t>1-2 years experience</t>
-  </si>
-  <si>
     <t>&lt;1 year experience</t>
   </si>
   <si>
@@ -97,6 +85,42 @@
   </si>
   <si>
     <t>Statistics</t>
+  </si>
+  <si>
+    <t>1+ years experience</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Classification &amp; regression, time series</t>
+  </si>
+  <si>
+    <t>K-Means, PCA</t>
+  </si>
+  <si>
+    <t>TensorFlow</t>
+  </si>
+  <si>
+    <t>HTML, CSS</t>
+  </si>
+  <si>
+    <t>Relational and NoSQL</t>
+  </si>
+  <si>
+    <t>Heroku, AWS</t>
+  </si>
+  <si>
+    <t>Pandas, Numpy</t>
+  </si>
+  <si>
+    <t>Matplotlib, Seaborn, Plotly, Shapley</t>
+  </si>
+  <si>
+    <t>Descriptive, inferential</t>
   </si>
 </sst>
 </file>
@@ -458,7 +482,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,13 +516,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -509,13 +533,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -526,13 +550,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -543,13 +567,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -560,13 +584,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -577,13 +601,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -594,13 +618,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -611,13 +635,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -628,13 +652,13 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -645,13 +669,13 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -662,13 +686,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -679,13 +703,13 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>